<commit_message>
Cleaning of Repository and Removing Extra Files - 20230601
</commit_message>
<xml_diff>
--- a/Dissertation 2023 - Bachelor Degree/EOS - Tweets 2022/EOS Sentiment Scores.xlsx
+++ b/Dissertation 2023 - Bachelor Degree/EOS - Tweets 2022/EOS Sentiment Scores.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e55a912db83fd400/Desktop/DissertationRepository2023/Dissertation 2023 - Bachelor Degree/EOS - Tweets 2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="800" documentId="8_{D8E6A5F6-E7BB-4102-ADC5-34B78C280278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36E82376-6744-44E8-B2C6-481DBE5FBD9A}"/>
+  <xr:revisionPtr revIDLastSave="807" documentId="8_{D8E6A5F6-E7BB-4102-ADC5-34B78C280278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{194A63FF-03BA-4440-B471-645222C22EE7}"/>
   <bookViews>
-    <workbookView xWindow="53535" yWindow="-1965" windowWidth="27060" windowHeight="21105" xr2:uid="{3FE3C018-F761-4452-BAD4-9E91D9E53B02}"/>
+    <workbookView xWindow="29760" yWindow="-1005" windowWidth="38700" windowHeight="15375" xr2:uid="{3FE3C018-F761-4452-BAD4-9E91D9E53B02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -637,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A8B9D35-5101-48E1-A0AA-BE397EB6158F}">
   <dimension ref="A1:X362"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A338" workbookViewId="0">
+      <selection activeCell="Q358" sqref="Q358"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11521,4 +11522,277 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE89922-6F14-44E7-9D42-ED409D45B056}">
+  <dimension ref="A1:CG1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:85" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <v>1</v>
+      </c>
+      <c r="F1">
+        <v>1</v>
+      </c>
+      <c r="G1">
+        <v>1</v>
+      </c>
+      <c r="H1">
+        <v>1</v>
+      </c>
+      <c r="I1">
+        <v>1</v>
+      </c>
+      <c r="J1">
+        <v>1</v>
+      </c>
+      <c r="K1">
+        <v>1</v>
+      </c>
+      <c r="L1">
+        <v>1</v>
+      </c>
+      <c r="M1">
+        <v>1</v>
+      </c>
+      <c r="N1">
+        <v>1</v>
+      </c>
+      <c r="O1">
+        <v>1</v>
+      </c>
+      <c r="P1">
+        <v>1</v>
+      </c>
+      <c r="Q1">
+        <v>1</v>
+      </c>
+      <c r="R1">
+        <v>1</v>
+      </c>
+      <c r="S1">
+        <v>1</v>
+      </c>
+      <c r="T1">
+        <v>1</v>
+      </c>
+      <c r="U1">
+        <v>1</v>
+      </c>
+      <c r="V1">
+        <v>1</v>
+      </c>
+      <c r="W1">
+        <v>1</v>
+      </c>
+      <c r="X1">
+        <v>1</v>
+      </c>
+      <c r="Y1">
+        <v>1</v>
+      </c>
+      <c r="Z1">
+        <v>1</v>
+      </c>
+      <c r="AA1">
+        <v>1</v>
+      </c>
+      <c r="AB1">
+        <v>1</v>
+      </c>
+      <c r="AC1">
+        <v>1</v>
+      </c>
+      <c r="AD1">
+        <v>1</v>
+      </c>
+      <c r="AE1">
+        <v>1</v>
+      </c>
+      <c r="AF1">
+        <v>1</v>
+      </c>
+      <c r="AG1">
+        <v>1</v>
+      </c>
+      <c r="AH1">
+        <v>1</v>
+      </c>
+      <c r="AI1">
+        <v>1</v>
+      </c>
+      <c r="AJ1">
+        <v>0</v>
+      </c>
+      <c r="AK1">
+        <v>0</v>
+      </c>
+      <c r="AL1">
+        <v>0</v>
+      </c>
+      <c r="AM1">
+        <v>0</v>
+      </c>
+      <c r="AN1">
+        <v>0</v>
+      </c>
+      <c r="AO1">
+        <v>0</v>
+      </c>
+      <c r="AP1">
+        <v>0</v>
+      </c>
+      <c r="AQ1">
+        <v>0</v>
+      </c>
+      <c r="AR1">
+        <v>0</v>
+      </c>
+      <c r="AS1">
+        <v>0</v>
+      </c>
+      <c r="AT1">
+        <v>0</v>
+      </c>
+      <c r="AU1">
+        <v>0</v>
+      </c>
+      <c r="AV1">
+        <v>0</v>
+      </c>
+      <c r="AW1">
+        <v>0</v>
+      </c>
+      <c r="AX1">
+        <v>0</v>
+      </c>
+      <c r="AY1">
+        <v>0</v>
+      </c>
+      <c r="AZ1">
+        <v>0</v>
+      </c>
+      <c r="BA1">
+        <v>0</v>
+      </c>
+      <c r="BB1">
+        <v>0</v>
+      </c>
+      <c r="BC1">
+        <v>0</v>
+      </c>
+      <c r="BD1">
+        <v>0</v>
+      </c>
+      <c r="BE1">
+        <v>0</v>
+      </c>
+      <c r="BF1">
+        <v>0</v>
+      </c>
+      <c r="BG1">
+        <v>0</v>
+      </c>
+      <c r="BH1">
+        <v>0</v>
+      </c>
+      <c r="BI1">
+        <v>0</v>
+      </c>
+      <c r="BJ1">
+        <v>0</v>
+      </c>
+      <c r="BK1">
+        <v>0</v>
+      </c>
+      <c r="BL1">
+        <v>0</v>
+      </c>
+      <c r="BM1">
+        <v>0</v>
+      </c>
+      <c r="BN1">
+        <v>0</v>
+      </c>
+      <c r="BO1">
+        <v>0</v>
+      </c>
+      <c r="BP1">
+        <v>0</v>
+      </c>
+      <c r="BQ1">
+        <v>0</v>
+      </c>
+      <c r="BR1">
+        <v>0</v>
+      </c>
+      <c r="BS1">
+        <v>0</v>
+      </c>
+      <c r="BT1">
+        <v>0</v>
+      </c>
+      <c r="BU1">
+        <v>0</v>
+      </c>
+      <c r="BV1">
+        <v>0</v>
+      </c>
+      <c r="BW1">
+        <v>0</v>
+      </c>
+      <c r="BX1">
+        <v>0</v>
+      </c>
+      <c r="BY1">
+        <v>0</v>
+      </c>
+      <c r="BZ1">
+        <v>0</v>
+      </c>
+      <c r="CA1">
+        <v>0</v>
+      </c>
+      <c r="CB1">
+        <v>0</v>
+      </c>
+      <c r="CC1">
+        <v>0</v>
+      </c>
+      <c r="CD1">
+        <v>0</v>
+      </c>
+      <c r="CE1">
+        <v>0</v>
+      </c>
+      <c r="CF1">
+        <v>0</v>
+      </c>
+      <c r="CG1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>